<commit_message>
filled in missing values for primary dataset using cleaned values from different dataset, data cleaning is complete
</commit_message>
<xml_diff>
--- a/data/01-raw_data/shanghai_population_distribution_1852_1942.xlsx
+++ b/data/01-raw_data/shanghai_population_distribution_1852_1942.xlsx
@@ -1,15 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woohuu_computer/R_projects/Shanghai_population/data/01-raw_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC65836-0365-7443-AD68-6C8307983D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4660" yWindow="500" windowWidth="35160" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$10</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$10</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$2:$A$10</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$D$2:$D$10</definedName>
+  </definedNames>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,8 +88,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +152,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +204,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -203,6 +238,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,9 +273,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -412,14 +449,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="285" zoomScaleNormal="285" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -453,7 +492,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -470,7 +509,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -487,7 +526,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -504,7 +543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -521,7 +560,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -529,7 +568,7 @@
         <v>53.9</v>
       </c>
       <c r="C7">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="D7">
         <v>13.9</v>
@@ -538,12 +577,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8">
-        <v>56.1</v>
+        <v>55.1</v>
       </c>
       <c r="C8">
         <v>31.4</v>
@@ -555,7 +594,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -572,12 +611,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10">
-        <v>37.8</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="C10">
         <v>40.4</v>

</xml_diff>